<commit_message>
Add support for zipfiles.
</commit_message>
<xml_diff>
--- a/anonymization-sheet.xlsx
+++ b/anonymization-sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joehe05\Documents\aida-pat-anonexcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joehe05\Documents\eraseme\aida-pat-anonexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6FA9B6-6E7D-4479-8EBF-DFAA97632BA7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5519DFA1-E5CD-4A0F-8AB2-BC0F09AEAEE9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11070" xr2:uid="{82B663A5-D320-4BF0-B0E4-C1F4FA1F5C31}"/>
+    <workbookView xWindow="285" yWindow="270" windowWidth="19200" windowHeight="11070" xr2:uid="{82B663A5-D320-4BF0-B0E4-C1F4FA1F5C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Prefix:</t>
   </si>
@@ -39,52 +39,72 @@
     <t>Digits:</t>
   </si>
   <si>
+    <t>AnonID</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Stain</t>
+  </si>
+  <si>
+    <t>Study parameter 1</t>
+  </si>
+  <si>
+    <t>Study parameter 2</t>
+  </si>
+  <si>
+    <t>Study parameter 3…</t>
+  </si>
+  <si>
+    <t>Example:</t>
+  </si>
+  <si>
+    <t>AIDA Pathology Anonymization Sheet</t>
+  </si>
+  <si>
+    <t>Howto:</t>
+  </si>
+  <si>
+    <t>3. Run aida-pat-anonexcel.py &lt;path to this file&gt; to fill out missing AnonID and AnonFile. Anonymized image files appear in subdirectory anon.</t>
+  </si>
+  <si>
+    <t>MYPROJ-</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Your data is now Pseudonymous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> because keys still exist that connect AnonIDs to Persons. Please verify that everything went as expected.</t>
+    </r>
+  </si>
+  <si>
+    <t>OrigFile</t>
+  </si>
+  <si>
     <t>Person</t>
   </si>
   <si>
-    <t>AnonID</t>
-  </si>
-  <si>
-    <t>Block</t>
-  </si>
-  <si>
-    <t>Stain</t>
-  </si>
-  <si>
-    <t>Study parameter 1</t>
-  </si>
-  <si>
-    <t>Study parameter 2</t>
-  </si>
-  <si>
-    <t>Study parameter 3…</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Example:</t>
-  </si>
-  <si>
-    <t>AnonFile</t>
-  </si>
-  <si>
-    <t>Image file</t>
-  </si>
-  <si>
-    <t>AIDA Pathology Anonymization Sheet</t>
-  </si>
-  <si>
-    <t>Howto:</t>
-  </si>
-  <si>
-    <t>3. Run aida-pat-anonexcel.py &lt;path to this file&gt; to fill out missing AnonID and AnonFile. Anonymized image files appear in subdirectory anon.</t>
-  </si>
-  <si>
-    <t>1. Put a copy of this file in a folder. Put image files in same folder or in subfolders named after Person.</t>
-  </si>
-  <si>
-    <t>2. Set Prefix for your study. If you want to assign a specific AnonID to a specific Person, type it out exactly on the first row where that Person occurs (eg DPL-JBR-123). New AnonIDs will be assigned sequentially from there on.</t>
+    <t>Status</t>
   </si>
   <si>
     <r>
@@ -109,7 +129,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: Delete all keys associating AnonIDs to Persons, including the </t>
+      <t xml:space="preserve">: Delete all keys associating AnonIDs to persons, including the </t>
     </r>
     <r>
       <rPr>
@@ -141,17 +161,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Image file</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> cells below, and any other identifiers that may exist. Obviously, </t>
+      <t>OrigFile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cells below and any other identifiers that may exist. Obviously, </t>
     </r>
     <r>
       <rPr>
@@ -176,33 +196,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">4. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Your data is now Pseudonymous.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Keys exist that connect AnonIDs to Persons. Please verify that everything went as expected.</t>
-    </r>
-  </si>
-  <si>
-    <t>MYPROJ-</t>
+    <t>1. Put a copy of this file in a folder. Put exported .zip files or folders named after Persons in same folder. Should contain BLOCK_STAIN (eg "A_HE") subfolders with one .svs file each in them.</t>
+  </si>
+  <si>
+    <t>2. Set Prefix for your study. AnonIDs are generated sequentially from the last AnonID given based on this prefix, or from 1 if none given (eg MYPROJ-001).</t>
   </si>
 </sst>
 </file>
@@ -590,124 +587,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D87FB2-CF59-4A73-A760-1BB024505B23}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="7" max="8" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="str">
+        <f>E9&amp;TEXT(1, REPT("0", E10))</f>
+        <v>MYPROJ-001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10">
+      <c r="D14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="str">
-        <f>C9&amp;TEXT(1, REPT("0", C10))</f>
-        <v>MYPROJ-001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Assign AnonID in Excel instead.
Prefix and Digits now dropped from the sheet. These are instead
taken from the AnonID on first Row, eg MYPROJ-0000 gives Prefix
MYPROJ- and Digits 4.

Assigning AnonIDs in Excel is completely fine if Persons are
required unique, because this allows user to type out the first
AnonID and then drag down to assign the rest sequentially.
</commit_message>
<xml_diff>
--- a/anonymization-sheet.xlsx
+++ b/anonymization-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joehe05\Documents\eraseme\aida-pat-anonexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5519DFA1-E5CD-4A0F-8AB2-BC0F09AEAEE9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84140065-E8F9-453E-AFD2-424F659AB39B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="270" windowWidth="19200" windowHeight="11070" xr2:uid="{82B663A5-D320-4BF0-B0E4-C1F4FA1F5C31}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15750" xr2:uid="{82B663A5-D320-4BF0-B0E4-C1F4FA1F5C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Prefix:</t>
-  </si>
-  <si>
-    <t>Digits:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>AnonID</t>
   </si>
@@ -57,21 +51,12 @@
     <t>Study parameter 3…</t>
   </si>
   <si>
-    <t>Example:</t>
-  </si>
-  <si>
     <t>AIDA Pathology Anonymization Sheet</t>
   </si>
   <si>
     <t>Howto:</t>
   </si>
   <si>
-    <t>3. Run aida-pat-anonexcel.py &lt;path to this file&gt; to fill out missing AnonID and AnonFile. Anonymized image files appear in subdirectory anon.</t>
-  </si>
-  <si>
-    <t>MYPROJ-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">4. </t>
     </r>
@@ -199,7 +184,10 @@
     <t>1. Put a copy of this file in a folder. Put exported .zip files or folders named after Persons in same folder. Should contain BLOCK_STAIN (eg "A_HE") subfolders with one .svs file each in them.</t>
   </si>
   <si>
-    <t>2. Set Prefix for your study. AnonIDs are generated sequentially from the last AnonID given based on this prefix, or from 1 if none given (eg MYPROJ-001).</t>
+    <t>2. Assign AnonIDs to your Persons. You can for example type in the first (eg "MYPROJ-001") and then drag down to number the rest sequentially.</t>
+  </si>
+  <si>
+    <t>3. Run aida-pat-anonexcel.py &lt;path to this file&gt; to check for mistakes, find and anonymize slides, and update this sheet to match.</t>
   </si>
 </sst>
 </file>
@@ -587,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D87FB2-CF59-4A73-A760-1BB024505B23}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,109 +591,79 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D10" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E10">
+      <c r="F9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="str">
-        <f>E9&amp;TEXT(1, REPT("0", E10))</f>
-        <v>MYPROJ-001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rename Parson -> Case. Documentation improvements.
</commit_message>
<xml_diff>
--- a/anonymization-sheet.xlsx
+++ b/anonymization-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joehe05\Documents\eraseme\aida-pat-anonexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84140065-E8F9-453E-AFD2-424F659AB39B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9F12E6-2749-4146-A233-12FED978AEAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15750" xr2:uid="{82B663A5-D320-4BF0-B0E4-C1F4FA1F5C31}"/>
+    <workbookView xWindow="4845" yWindow="4335" windowWidth="28800" windowHeight="15750" xr2:uid="{82B663A5-D320-4BF0-B0E4-C1F4FA1F5C31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>AnonID</t>
   </si>
@@ -57,8 +57,32 @@
     <t>Howto:</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">4. </t>
+    <t>OrigFile</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>1. Put a copy of this file in a folder.</t>
+  </si>
+  <si>
+    <t>3. Assign increasing AnonIDs to your Cases, for example by typing in the one on the first row (eg "MYPROJ-001") and then dragging down to number the rest sequentially.</t>
+  </si>
+  <si>
+    <t>2. List Cases to anonymize below. Use the same .zip filenames or folder names as you get when exporting cases from the PACS, preferably in random order.</t>
+  </si>
+  <si>
+    <t>4. Export cases and put in same folder. If using folders, these should have BLOCK_STAIN subfolders cotaining one .svs or .ndpi file each. Don't fill up more than half your available storage.</t>
+  </si>
+  <si>
+    <t>5. Run aida-pat-anonexcel.py on this file to check for mistakes, anonymize slides, and update this sheet to match.</t>
+  </si>
+  <si>
+    <t>8. Export to research system. Delete exported cases and anonymized images. Repeat from 4 until all cases have been processed.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6. </t>
     </r>
     <r>
       <rPr>
@@ -69,31 +93,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Your data is now Pseudonymous</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> because keys still exist that connect AnonIDs to Persons. Please verify that everything went as expected.</t>
-    </r>
-  </si>
-  <si>
-    <t>OrigFile</t>
-  </si>
-  <si>
-    <t>Person</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5. </t>
+      <t>Your output data is now Pseudonymous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> because keys still exist that connect AnonIDs to persons. Take this moment to verify that everything went as expected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">7. </t>
     </r>
     <r>
       <rPr>
@@ -125,7 +140,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Person</t>
+      <t>Case</t>
     </r>
     <r>
       <rPr>
@@ -181,13 +196,7 @@
     </r>
   </si>
   <si>
-    <t>1. Put a copy of this file in a folder. Put exported .zip files or folders named after Persons in same folder. Should contain BLOCK_STAIN (eg "A_HE") subfolders with one .svs file each in them.</t>
-  </si>
-  <si>
-    <t>2. Assign AnonIDs to your Persons. You can for example type in the first (eg "MYPROJ-001") and then drag down to number the rest sequentially.</t>
-  </si>
-  <si>
-    <t>3. Run aida-pat-anonexcel.py &lt;path to this file&gt; to check for mistakes, find and anonymize slides, and update this sheet to match.</t>
+    <t>Case</t>
   </si>
 </sst>
 </file>
@@ -575,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D87FB2-CF59-4A73-A760-1BB024505B23}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,69 +610,84 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>